<commit_message>
Changing names to portuguese
</commit_message>
<xml_diff>
--- a/inputs.xlsx
+++ b/inputs.xlsx
@@ -1,20 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brene\Dropbox\shift_manager\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFBEEE8A-6E8D-4936-9A42-1F7F0DD71D46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39B62EAF-A464-4E74-80CD-2E002F4B42D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="employees" sheetId="1" r:id="rId1"/>
-    <sheet name="areas" sheetId="2" r:id="rId2"/>
+    <sheet name="funcionários" sheetId="1" r:id="rId1"/>
+    <sheet name="folgas" sheetId="6" r:id="rId2"/>
+    <sheet name="áreas" sheetId="2" r:id="rId3"/>
+    <sheet name="mês" sheetId="3" r:id="rId4"/>
+    <sheet name="condições" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,8 +36,35 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={95C69F06-1F8E-45D4-8726-04707BCE9F45}</author>
+    <author>tc={2956268A-A1D4-4A20-AD11-190863ED994F}</author>
+  </authors>
+  <commentList>
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{95C69F06-1F8E-45D4-8726-04707BCE9F45}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Use "_" for designating subareas only</t>
+      </text>
+    </comment>
+    <comment ref="I1" authorId="1" shapeId="0" xr:uid="{2956268A-A1D4-4A20-AD11-190863ED994F}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    E.g. 2023-09-07, 2023-09-15</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="69">
   <si>
     <t>Nome</t>
   </si>
@@ -69,9 +99,6 @@
     <t>Lilian</t>
   </si>
   <si>
-    <t>Marcela</t>
-  </si>
-  <si>
     <t>Leticia</t>
   </si>
   <si>
@@ -90,9 +117,6 @@
     <t>Iara</t>
   </si>
   <si>
-    <t>Henrique</t>
-  </si>
-  <si>
     <t>Maria</t>
   </si>
   <si>
@@ -108,18 +132,6 @@
     <t>Giovanna</t>
   </si>
   <si>
-    <t>Joyce</t>
-  </si>
-  <si>
-    <t>Area</t>
-  </si>
-  <si>
-    <t>Duracao</t>
-  </si>
-  <si>
-    <t>Periodo</t>
-  </si>
-  <si>
     <t>N_Residentes</t>
   </si>
   <si>
@@ -129,63 +141,36 @@
     <t>Balancear</t>
   </si>
   <si>
-    <t>Obrigatorio</t>
-  </si>
-  <si>
     <t>Exceto</t>
   </si>
   <si>
     <t>Plantao_Noturno</t>
   </si>
   <si>
-    <t>E</t>
-  </si>
-  <si>
-    <t>MON, TUE, WED, THU, FRI, SAT, SUN</t>
-  </si>
-  <si>
     <t>Plantao_Diurno</t>
   </si>
   <si>
     <t>M</t>
   </si>
   <si>
-    <t>SAT, SUN</t>
-  </si>
-  <si>
     <t>Puerperio_Manha1</t>
   </si>
   <si>
-    <t>MON, WED</t>
-  </si>
-  <si>
     <t>Puerperio_Manha2</t>
   </si>
   <si>
-    <t>TUE, THU, FRI</t>
-  </si>
-  <si>
     <t>Puerperio_Manha_Ambulatorio</t>
   </si>
   <si>
     <t>Gineco_Manha1</t>
   </si>
   <si>
-    <t>MON, THU</t>
-  </si>
-  <si>
     <t>Gineco_Manha2</t>
   </si>
   <si>
-    <t>WED</t>
-  </si>
-  <si>
     <t>Gineco_Manha3</t>
   </si>
   <si>
-    <t>FRI</t>
-  </si>
-  <si>
     <t>Gineco_Manha_Cirurgia1</t>
   </si>
   <si>
@@ -195,35 +180,104 @@
     <t>Gineco_Manha_Cirurgia3</t>
   </si>
   <si>
-    <t>TUE</t>
-  </si>
-  <si>
-    <t>MON, TUE, WED, THU, FRI</t>
-  </si>
-  <si>
     <t>Ambulatorio_Manha</t>
   </si>
   <si>
     <t>Ambulatorio_Tarde</t>
   </si>
   <si>
-    <t>A</t>
-  </si>
-  <si>
     <t>Permanencia2</t>
   </si>
   <si>
-    <t>MON, WED, THU, FRI</t>
-  </si>
-  <si>
     <t>Permanencia3</t>
+  </si>
+  <si>
+    <t>Camila</t>
+  </si>
+  <si>
+    <t>Vitória</t>
+  </si>
+  <si>
+    <t>EvolucaoFeriado</t>
+  </si>
+  <si>
+    <t>2023-09-14, 2023-09-21, 2023-09-28</t>
+  </si>
+  <si>
+    <t>2023-09-07</t>
+  </si>
+  <si>
+    <t>AltoRisco</t>
+  </si>
+  <si>
+    <t>SalaParto</t>
+  </si>
+  <si>
+    <t>BaixoRisco</t>
+  </si>
+  <si>
+    <t>Datas</t>
+  </si>
+  <si>
+    <t>MaxTurnos</t>
+  </si>
+  <si>
+    <t>Área</t>
+  </si>
+  <si>
+    <t>Duração</t>
+  </si>
+  <si>
+    <t>Período</t>
+  </si>
+  <si>
+    <t>Obrigatório</t>
+  </si>
+  <si>
+    <t>TER</t>
+  </si>
+  <si>
+    <t>SEG, QUA</t>
+  </si>
+  <si>
+    <t>QUA</t>
+  </si>
+  <si>
+    <t>SEG, QUI</t>
+  </si>
+  <si>
+    <t>QUI</t>
+  </si>
+  <si>
+    <t>TER, QUI, SEX</t>
+  </si>
+  <si>
+    <t>SEX</t>
+  </si>
+  <si>
+    <t>SEG, TER, QUA, QUI, SEX</t>
+  </si>
+  <si>
+    <t>SEG, QUA, QUI, SEX</t>
+  </si>
+  <si>
+    <t>SEG, TER, QUA, QUI, SEX, SAB, DOM</t>
+  </si>
+  <si>
+    <t>SAB, DOM</t>
+  </si>
+  <si>
+    <t>T</t>
+  </si>
+  <si>
+    <t>N</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -354,6 +408,14 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -700,12 +762,18 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -773,6 +841,12 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="Brener Lélis" id="{D69F0609-D041-443E-BE14-603F0DF32961}" userId="c73481bbb311cf03" providerId="Windows Live"/>
+</personList>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1070,12 +1144,23 @@
 </a:theme>
 </file>
 
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="B1" dT="2023-08-02T13:37:24.67" personId="{D69F0609-D041-443E-BE14-603F0DF32961}" id="{95C69F06-1F8E-45D4-8726-04707BCE9F45}">
+    <text>Use "_" for designating subareas only</text>
+  </threadedComment>
+  <threadedComment ref="I1" dT="2023-08-02T02:28:35.91" personId="{D69F0609-D041-443E-BE14-603F0DF32961}" id="{2956268A-A1D4-4A20-AD11-190863ED994F}">
+    <text>E.g. 2023-09-07, 2023-09-15</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+    <sheetView zoomScale="93" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1089,28 +1174,28 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>15</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>3</v>
+        <v>47</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>5</v>
+        <v>48</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>6</v>
@@ -1119,70 +1204,70 @@
         <v>7</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>8</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B2" s="1"/>
+        <v>42</v>
+      </c>
+      <c r="B2" s="1">
+        <v>1</v>
+      </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
+      <c r="E2" s="1">
+        <v>1</v>
+      </c>
+      <c r="F2" s="1">
+        <v>1</v>
+      </c>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
-      <c r="I2" s="1">
-        <v>1</v>
-      </c>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1">
+        <v>1</v>
+      </c>
+      <c r="K2" s="1">
+        <v>1</v>
+      </c>
       <c r="L2" s="1"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B3" s="1">
-        <v>1</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
-      <c r="H3" s="1">
-        <v>1</v>
-      </c>
-      <c r="I3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1">
+        <v>1</v>
+      </c>
       <c r="J3" s="1"/>
-      <c r="K3" s="1">
-        <v>1</v>
-      </c>
+      <c r="K3" s="1"/>
       <c r="L3" s="1"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B4" s="1">
         <v>1</v>
       </c>
-      <c r="C4" s="1">
-        <v>1</v>
-      </c>
-      <c r="D4" s="1">
-        <v>1</v>
-      </c>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
+      <c r="H4" s="1">
+        <v>1</v>
+      </c>
       <c r="I4" s="1"/>
-      <c r="J4" s="1">
-        <v>1</v>
-      </c>
+      <c r="J4" s="1"/>
       <c r="K4" s="1">
         <v>1</v>
       </c>
@@ -1190,19 +1275,19 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B5" s="1">
         <v>1</v>
       </c>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1">
-        <v>1</v>
-      </c>
-      <c r="F5" s="1">
-        <v>1</v>
-      </c>
+      <c r="C5" s="1">
+        <v>1</v>
+      </c>
+      <c r="D5" s="1">
+        <v>1</v>
+      </c>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
@@ -1216,18 +1301,20 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B6" s="1">
         <v>1</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1">
-        <v>1</v>
-      </c>
+      <c r="E6" s="1">
+        <v>1</v>
+      </c>
+      <c r="F6" s="1">
+        <v>1</v>
+      </c>
+      <c r="G6" s="1"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
       <c r="J6" s="1">
@@ -1240,20 +1327,18 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B7" s="1">
         <v>1</v>
       </c>
-      <c r="C7" s="1">
-        <v>1</v>
-      </c>
-      <c r="D7" s="1">
-        <v>1</v>
-      </c>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
+      <c r="G7" s="1">
+        <v>1</v>
+      </c>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
       <c r="J7" s="1">
@@ -1271,14 +1356,14 @@
       <c r="B8" s="1">
         <v>1</v>
       </c>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1">
-        <v>1</v>
-      </c>
-      <c r="F8" s="1">
-        <v>1</v>
-      </c>
+      <c r="C8" s="1">
+        <v>1</v>
+      </c>
+      <c r="D8" s="1">
+        <v>1</v>
+      </c>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
@@ -1292,7 +1377,7 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="B9" s="1">
         <v>1</v>
@@ -1318,29 +1403,21 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>16</v>
-      </c>
-      <c r="B10" s="1">
-        <v>1</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
-      <c r="E10" s="1">
-        <v>1</v>
-      </c>
-      <c r="F10" s="1">
-        <v>1</v>
-      </c>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
-      <c r="J10" s="1">
-        <v>1</v>
-      </c>
-      <c r="K10" s="1">
-        <v>1</v>
-      </c>
-      <c r="L10" s="1"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="1"/>
+      <c r="L10" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
@@ -1353,72 +1430,69 @@
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
+      <c r="I11" s="1">
+        <v>1</v>
+      </c>
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
-      <c r="L11" s="1">
-        <v>1</v>
-      </c>
+      <c r="L11" s="1"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>11</v>
-      </c>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
+        <v>16</v>
+      </c>
+      <c r="B12" s="1">
+        <v>1</v>
+      </c>
+      <c r="C12" s="1">
+        <v>1</v>
+      </c>
+      <c r="D12" s="1">
+        <v>1</v>
+      </c>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
-      <c r="I12" s="1">
-        <v>1</v>
-      </c>
-      <c r="J12" s="1"/>
-      <c r="K12" s="1"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1">
+        <v>1</v>
+      </c>
+      <c r="K12" s="1">
+        <v>1</v>
+      </c>
       <c r="L12" s="1"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>43</v>
       </c>
       <c r="B13" s="1">
         <v>1</v>
       </c>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
+      <c r="E13" s="1">
+        <v>1</v>
+      </c>
+      <c r="F13" s="1">
+        <v>1</v>
+      </c>
       <c r="G13" s="1"/>
-      <c r="H13" s="1">
-        <v>1</v>
-      </c>
+      <c r="H13" s="1"/>
       <c r="I13" s="1"/>
-      <c r="J13" s="1"/>
+      <c r="J13" s="1">
+        <v>1</v>
+      </c>
       <c r="K13" s="1">
         <v>1</v>
       </c>
       <c r="L13" s="1"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
-        <v>17</v>
-      </c>
-      <c r="B14" s="1">
-        <v>1</v>
-      </c>
-      <c r="E14">
-        <v>1</v>
-      </c>
-      <c r="F14">
-        <v>1</v>
-      </c>
-      <c r="J14" s="1">
-        <v>1</v>
-      </c>
-      <c r="K14" s="1">
-        <v>1</v>
-      </c>
+      <c r="B14" s="1"/>
+      <c r="J14" s="1"/>
+      <c r="K14" s="1"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:L33">
@@ -1431,67 +1505,169 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6501031-25F1-4A38-BB75-66883E67F2F3}">
-  <dimension ref="A1:I20"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76EC4CF4-1F5E-49DE-AA5D-A45D532E114B}">
+  <dimension ref="A1:B13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" t="str">
+        <f>funcionários!A1</f>
+        <v>Nome</v>
+      </c>
+      <c r="B1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="str">
+        <f>funcionários!A2</f>
+        <v>Camila</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" t="str">
+        <f>funcionários!A3</f>
+        <v>Maria</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" t="str">
+        <f>funcionários!A4</f>
+        <v>Jessika</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" t="str">
+        <f>funcionários!A5</f>
+        <v>Isabelle</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" t="str">
+        <f>funcionários!A6</f>
+        <v>Rafaela</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" t="str">
+        <f>funcionários!A7</f>
+        <v>Giovanna</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" t="str">
+        <f>funcionários!A8</f>
+        <v>Ana Luiza</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9" t="str">
+        <f>funcionários!A9</f>
+        <v>Leticia</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10" t="str">
+        <f>funcionários!A10</f>
+        <v>Duda</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A11" t="str">
+        <f>funcionários!A11</f>
+        <v>Lilian</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A12" t="str">
+        <f>funcionários!A12</f>
+        <v>Iara</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A13" t="str">
+        <f>funcionários!A13</f>
+        <v>Vitória</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6501031-25F1-4A38-BB75-66883E67F2F3}">
+  <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:I26"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="27.7265625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20.6328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.36328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.7265625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="31.08984375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.90625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="30.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:9" ht="21" x14ac:dyDescent="0.5">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="I1" s="4" t="s">
         <v>25</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C2" s="1">
         <v>12</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>34</v>
+        <v>68</v>
       </c>
       <c r="E2" s="1">
         <v>2</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>35</v>
+        <v>65</v>
       </c>
       <c r="G2" s="1">
         <v>1</v>
@@ -1503,22 +1679,22 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C3" s="1">
         <v>12</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="E3" s="1">
         <v>2</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>38</v>
+        <v>66</v>
       </c>
       <c r="G3" s="1">
         <v>1</v>
@@ -1530,7 +1706,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>1</v>
@@ -1539,13 +1715,13 @@
         <v>5</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="E4" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>40</v>
+        <v>57</v>
       </c>
       <c r="G4" s="1">
         <v>0</v>
@@ -1553,11 +1729,13 @@
       <c r="H4" s="1">
         <v>1</v>
       </c>
-      <c r="I4" s="2"/>
+      <c r="I4" s="2" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>1</v>
@@ -1566,13 +1744,13 @@
         <v>5</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="E5" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>42</v>
+        <v>61</v>
       </c>
       <c r="G5" s="1">
         <v>0</v>
@@ -1580,26 +1758,28 @@
       <c r="H5" s="1">
         <v>1</v>
       </c>
-      <c r="I5" s="2"/>
+      <c r="I5" s="2" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C6" s="1">
         <v>8</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="E6" s="1">
         <v>1</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>42</v>
+        <v>61</v>
       </c>
       <c r="G6" s="1">
         <v>1</v>
@@ -1607,11 +1787,13 @@
       <c r="H6" s="1">
         <v>1</v>
       </c>
-      <c r="I6" s="2"/>
+      <c r="I6" s="2" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>2</v>
@@ -1620,13 +1802,13 @@
         <v>5</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="E7" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>45</v>
+        <v>59</v>
       </c>
       <c r="G7" s="1">
         <v>0</v>
@@ -1634,11 +1816,13 @@
       <c r="H7" s="1">
         <v>1</v>
       </c>
-      <c r="I7" s="2"/>
+      <c r="I7" s="2" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>2</v>
@@ -1647,13 +1831,13 @@
         <v>5</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="E8" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
       <c r="G8" s="1">
         <v>0</v>
@@ -1661,11 +1845,13 @@
       <c r="H8" s="1">
         <v>1</v>
       </c>
-      <c r="I8" s="2"/>
+      <c r="I8" s="2" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>2</v>
@@ -1674,13 +1860,13 @@
         <v>5</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="E9" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>49</v>
+        <v>62</v>
       </c>
       <c r="G9" s="1">
         <v>0</v>
@@ -1688,26 +1874,28 @@
       <c r="H9" s="1">
         <v>1</v>
       </c>
-      <c r="I9" s="2"/>
+      <c r="I9" s="2" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
-        <v>50</v>
+        <v>35</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C10" s="1">
         <v>9</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="E10" s="1">
         <v>1</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
       <c r="G10" s="1">
         <v>1</v>
@@ -1715,26 +1903,28 @@
       <c r="H10" s="1">
         <v>1</v>
       </c>
-      <c r="I10" s="2"/>
+      <c r="I10" s="2" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
-        <v>51</v>
+        <v>36</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C11" s="1">
         <v>9</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="E11" s="1">
         <v>2</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>45</v>
+        <v>59</v>
       </c>
       <c r="G11" s="1">
         <v>1</v>
@@ -1742,26 +1932,28 @@
       <c r="H11" s="1">
         <v>1</v>
       </c>
-      <c r="I11" s="2"/>
+      <c r="I11" s="2" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
-        <v>52</v>
+        <v>37</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C12" s="1">
         <v>9</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="E12" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="G12" s="1">
         <v>1</v>
@@ -1769,26 +1961,28 @@
       <c r="H12" s="1">
         <v>1</v>
       </c>
-      <c r="I12" s="2"/>
+      <c r="I12" s="2" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>3</v>
+        <v>47</v>
       </c>
       <c r="C13" s="1">
         <v>5</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="E13" s="1">
         <v>1</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>54</v>
+        <v>63</v>
       </c>
       <c r="G13" s="1">
         <v>0</v>
@@ -1796,11 +1990,13 @@
       <c r="H13" s="1">
         <v>1</v>
       </c>
-      <c r="I13" s="2"/>
+      <c r="I13" s="2" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
-        <v>55</v>
+        <v>38</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>4</v>
@@ -1809,13 +2005,13 @@
         <v>4</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="E14" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>54</v>
+        <v>63</v>
       </c>
       <c r="G14" s="1">
         <v>0</v>
@@ -1823,11 +2019,13 @@
       <c r="H14" s="1">
         <v>1</v>
       </c>
-      <c r="I14" s="2"/>
+      <c r="I14" s="2" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
-        <v>56</v>
+        <v>39</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>4</v>
@@ -1836,13 +2034,13 @@
         <v>4</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>57</v>
+        <v>67</v>
       </c>
       <c r="E15" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>54</v>
+        <v>63</v>
       </c>
       <c r="G15" s="1">
         <v>0</v>
@@ -1850,26 +2048,28 @@
       <c r="H15" s="1">
         <v>0</v>
       </c>
-      <c r="I15" s="2"/>
+      <c r="I15" s="2" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>5</v>
+        <v>48</v>
       </c>
       <c r="C16" s="1">
         <v>12</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="E16" s="1">
         <v>2</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>54</v>
+        <v>63</v>
       </c>
       <c r="G16" s="1">
         <v>0</v>
@@ -1881,7 +2081,7 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
-        <v>58</v>
+        <v>40</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>6</v>
@@ -1890,13 +2090,13 @@
         <v>4.5</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>57</v>
+        <v>67</v>
       </c>
       <c r="E17" s="1">
         <v>2</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="G17" s="1">
         <v>1</v>
@@ -1904,11 +2104,13 @@
       <c r="H17" s="1">
         <v>1</v>
       </c>
-      <c r="I17" s="2"/>
+      <c r="I17" s="2" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
-        <v>60</v>
+        <v>41</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>6</v>
@@ -1917,13 +2119,13 @@
         <v>4.5</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>57</v>
+        <v>67</v>
       </c>
       <c r="E18" s="1">
         <v>3</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="G18" s="1">
         <v>1</v>
@@ -1931,7 +2133,9 @@
       <c r="H18" s="1">
         <v>1</v>
       </c>
-      <c r="I18" s="2"/>
+      <c r="I18" s="2" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
@@ -1944,13 +2148,13 @@
         <v>5</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="E19" s="1">
         <v>2</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>38</v>
+        <v>66</v>
       </c>
       <c r="G19" s="1">
         <v>1</v>
@@ -1965,19 +2169,19 @@
         <v>8</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>8</v>
+        <v>49</v>
       </c>
       <c r="C20" s="1">
         <v>12</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="E20" s="1">
         <v>1</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>54</v>
+        <v>63</v>
       </c>
       <c r="G20" s="1">
         <v>0</v>
@@ -1986,6 +2190,148 @@
         <v>1</v>
       </c>
       <c r="I20" s="2"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A21" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C21" s="1">
+        <v>5</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E21" s="1">
+        <v>2</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="G21" s="1">
+        <v>1</v>
+      </c>
+      <c r="H21" s="1">
+        <v>1</v>
+      </c>
+      <c r="I21" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC5A3A86-226E-4815-90B2-75AB00A444C5}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02A25F96-0905-42BF-A354-862CB855866B}">
+  <dimension ref="A1:B21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="20.6328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" s="1"/>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" s="1"/>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" s="1"/>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" s="1"/>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" s="1"/>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" s="1"/>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9" s="1"/>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10" s="1"/>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A11" s="1"/>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A12" s="1"/>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A13" s="1"/>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A14" s="1"/>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A15" s="1"/>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A16" s="1"/>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A17" s="1"/>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A18" s="1"/>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A19" s="1"/>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A20" s="1"/>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A21" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Filling shifts in reverse now
</commit_message>
<xml_diff>
--- a/inputs.xlsx
+++ b/inputs.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brene\Dropbox\shift_manager\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39B62EAF-A464-4E74-80CD-2E002F4B42D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{739E2969-933A-44C5-BCE5-441A67E7DC41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="74">
   <si>
     <t>Nome</t>
   </si>
@@ -99,9 +99,6 @@
     <t>Lilian</t>
   </si>
   <si>
-    <t>Leticia</t>
-  </si>
-  <si>
     <t>Plantao</t>
   </si>
   <si>
@@ -117,9 +114,6 @@
     <t>Iara</t>
   </si>
   <si>
-    <t>Maria</t>
-  </si>
-  <si>
     <t>Jessika</t>
   </si>
   <si>
@@ -129,9 +123,6 @@
     <t>Rafaela</t>
   </si>
   <si>
-    <t>Giovanna</t>
-  </si>
-  <si>
     <t>N_Residentes</t>
   </si>
   <si>
@@ -195,18 +186,6 @@
     <t>Camila</t>
   </si>
   <si>
-    <t>Vitória</t>
-  </si>
-  <si>
-    <t>EvolucaoFeriado</t>
-  </si>
-  <si>
-    <t>2023-09-14, 2023-09-21, 2023-09-28</t>
-  </si>
-  <si>
-    <t>2023-09-07</t>
-  </si>
-  <si>
     <t>AltoRisco</t>
   </si>
   <si>
@@ -246,9 +225,6 @@
     <t>SEG, QUI</t>
   </si>
   <si>
-    <t>QUI</t>
-  </si>
-  <si>
     <t>TER, QUI, SEX</t>
   </si>
   <si>
@@ -261,9 +237,6 @@
     <t>SEG, QUA, QUI, SEX</t>
   </si>
   <si>
-    <t>SEG, TER, QUA, QUI, SEX, SAB, DOM</t>
-  </si>
-  <si>
     <t>SAB, DOM</t>
   </si>
   <si>
@@ -271,6 +244,48 @@
   </si>
   <si>
     <t>N</t>
+  </si>
+  <si>
+    <t>Henrique</t>
+  </si>
+  <si>
+    <t>Giovana</t>
+  </si>
+  <si>
+    <t>Joyce</t>
+  </si>
+  <si>
+    <t>Vitoria</t>
+  </si>
+  <si>
+    <t>Marcela</t>
+  </si>
+  <si>
+    <t>2023-10-12</t>
+  </si>
+  <si>
+    <t>SEG</t>
+  </si>
+  <si>
+    <t>TER, QUA, QUI, SEX, SAB, DOM</t>
+  </si>
+  <si>
+    <t>Plantao_Noturno_Seg</t>
+  </si>
+  <si>
+    <t>2023-10-13 (N), 2023-10-14 (MTN), 2023-10-15 (MTN), 2023-10-11 (T)</t>
+  </si>
+  <si>
+    <t>2023-10-07 (MTN), 2023-10-08 (M)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023-10-01 (MTN), 2023-10-27 (N), 2023-10-28 (MTN), 2023-10-29 (MTN) </t>
+  </si>
+  <si>
+    <t>2023-10-01(MTN), 2023-10-13 (N), 2023-10-14 (MTN), 2023-10-15 (MTN)</t>
+  </si>
+  <si>
+    <t>2023-10-11 (T)</t>
   </si>
 </sst>
 </file>
@@ -762,7 +777,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -773,6 +788,9 @@
     </xf>
     <xf numFmtId="49" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1160,12 +1178,12 @@
   <dimension ref="A1:L14"/>
   <sheetViews>
     <sheetView zoomScale="93" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16" customWidth="1"/>
     <col min="2" max="12" width="20.6328125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1174,28 +1192,28 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>14</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>6</v>
@@ -1204,12 +1222,12 @@
         <v>7</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>42</v>
+        <v>60</v>
       </c>
       <c r="B2" s="1">
         <v>1</v>
@@ -1235,7 +1253,7 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -1253,7 +1271,7 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B4" s="1">
         <v>1</v>
@@ -1275,7 +1293,7 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B5" s="1">
         <v>1</v>
@@ -1301,7 +1319,7 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>20</v>
+        <v>61</v>
       </c>
       <c r="B6" s="1">
         <v>1</v>
@@ -1327,7 +1345,7 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="B7" s="1">
         <v>1</v>
@@ -1351,7 +1369,7 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>62</v>
       </c>
       <c r="B8" s="1">
         <v>1</v>
@@ -1377,7 +1395,7 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B9" s="1">
         <v>1</v>
@@ -1403,7 +1421,7 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>15</v>
+        <v>63</v>
       </c>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -1421,7 +1439,7 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -1439,19 +1457,19 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B12" s="1">
         <v>1</v>
       </c>
-      <c r="C12" s="1">
-        <v>1</v>
-      </c>
-      <c r="D12" s="1">
-        <v>1</v>
-      </c>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1">
+        <v>1</v>
+      </c>
+      <c r="F12" s="1">
+        <v>1</v>
+      </c>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
@@ -1465,7 +1483,7 @@
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>43</v>
+        <v>64</v>
       </c>
       <c r="B13" s="1">
         <v>1</v>
@@ -1490,12 +1508,15 @@
       <c r="L13" s="1"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="B14" s="1"/>
-      <c r="J14" s="1"/>
-      <c r="K14" s="1"/>
+      <c r="A14" t="s">
+        <v>39</v>
+      </c>
+      <c r="L14">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B2:L33">
+  <conditionalFormatting sqref="B2:L32">
     <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",B2)))</formula>
     </cfRule>
@@ -1506,94 +1527,134 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76EC4CF4-1F5E-49DE-AA5D-A45D532E114B}">
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="8.7265625" customWidth="1"/>
+    <col min="2" max="2" width="30.453125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="str">
         <f>funcionários!A1</f>
         <v>Nome</v>
       </c>
-      <c r="B1" t="s">
-        <v>50</v>
+      <c r="B1" s="2" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="str">
         <f>funcionários!A2</f>
-        <v>Camila</v>
-      </c>
+        <v>Henrique</v>
+      </c>
+      <c r="B2" s="5"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="str">
         <f>funcionários!A3</f>
-        <v>Maria</v>
-      </c>
+        <v>Jessika</v>
+      </c>
+      <c r="B3" s="5"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="str">
         <f>funcionários!A4</f>
-        <v>Jessika</v>
-      </c>
+        <v>Isabelle</v>
+      </c>
+      <c r="B4" s="5"/>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="str">
         <f>funcionários!A5</f>
-        <v>Isabelle</v>
-      </c>
+        <v>Rafaela</v>
+      </c>
+      <c r="B5" s="5"/>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="str">
         <f>funcionários!A6</f>
-        <v>Rafaela</v>
+        <v>Giovana</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="str">
         <f>funcionários!A7</f>
-        <v>Giovanna</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+        <v>Ana Luiza</v>
+      </c>
+      <c r="B7" s="5"/>
+    </row>
+    <row r="8" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A8" t="str">
         <f>funcionários!A8</f>
-        <v>Ana Luiza</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+        <v>Joyce</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A9" t="str">
         <f>funcionários!A9</f>
-        <v>Leticia</v>
+        <v>Lilian</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="str">
         <f>funcionários!A10</f>
-        <v>Duda</v>
-      </c>
+        <v>Vitoria</v>
+      </c>
+      <c r="B10" s="5"/>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="str">
         <f>funcionários!A11</f>
-        <v>Lilian</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+        <v>Duda</v>
+      </c>
+      <c r="B11" s="5"/>
+    </row>
+    <row r="12" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A12" t="str">
         <f>funcionários!A12</f>
         <v>Iara</v>
       </c>
+      <c r="B12" s="5" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="str">
         <f>funcionários!A13</f>
-        <v>Vitória</v>
-      </c>
+        <v>Marcela</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A14" t="str">
+        <f>funcionários!A14</f>
+        <v>Camila</v>
+      </c>
+      <c r="B14" s="5"/>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A15">
+        <f>funcionários!A15</f>
+        <v>0</v>
+      </c>
+      <c r="B15" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1602,10 +1663,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6501031-25F1-4A38-BB75-66883E67F2F3}">
-  <dimension ref="A1:I21"/>
+  <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1626,48 +1687,48 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="E1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="I1" s="4" t="s">
         <v>22</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C2" s="1">
         <v>12</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="E2" s="1">
         <v>2</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="G2" s="1">
         <v>1</v>
@@ -1679,19 +1740,19 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>27</v>
+        <v>68</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C3" s="1">
         <v>12</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>28</v>
+        <v>59</v>
       </c>
       <c r="E3" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>66</v>
@@ -1706,36 +1767,34 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="C4" s="1">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E4" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>57</v>
       </c>
       <c r="G4" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H4" s="1">
         <v>1</v>
       </c>
-      <c r="I4" s="2" t="s">
-        <v>46</v>
-      </c>
+      <c r="I4" s="2"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>1</v>
@@ -1744,13 +1803,13 @@
         <v>5</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E5" s="1">
         <v>3</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="G5" s="1">
         <v>0</v>
@@ -1759,70 +1818,70 @@
         <v>1</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>46</v>
+        <v>65</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="C6" s="1">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E6" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="G6" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H6" s="1">
         <v>1</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>46</v>
+        <v>65</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="C7" s="1">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E7" s="1">
         <v>1</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="G7" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H7" s="1">
         <v>1</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>46</v>
+        <v>65</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>2</v>
@@ -1831,13 +1890,13 @@
         <v>5</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E8" s="1">
         <v>2</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="G8" s="1">
         <v>0</v>
@@ -1846,12 +1905,12 @@
         <v>1</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>46</v>
+        <v>65</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>2</v>
@@ -1860,13 +1919,13 @@
         <v>5</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E9" s="1">
         <v>3</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="G9" s="1">
         <v>0</v>
@@ -1875,56 +1934,56 @@
         <v>1</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>46</v>
+        <v>65</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="C10" s="1">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E10" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="G10" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H10" s="1">
         <v>1</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>46</v>
+        <v>65</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C11" s="1">
         <v>9</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E11" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="G11" s="1">
         <v>1</v>
@@ -1933,27 +1992,27 @@
         <v>1</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>46</v>
+        <v>65</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C12" s="1">
         <v>9</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E12" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="G12" s="1">
         <v>1</v>
@@ -1962,56 +2021,56 @@
         <v>1</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>46</v>
+        <v>65</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
-        <v>3</v>
+        <v>34</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>47</v>
+        <v>13</v>
       </c>
       <c r="C13" s="1">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E13" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>63</v>
+        <v>49</v>
       </c>
       <c r="G13" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H13" s="1">
         <v>1</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>46</v>
+        <v>65</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>4</v>
+        <v>40</v>
       </c>
       <c r="C14" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E14" s="1">
         <v>1</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="G14" s="1">
         <v>0</v>
@@ -2020,12 +2079,12 @@
         <v>1</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>46</v>
+        <v>65</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>4</v>
@@ -2034,83 +2093,83 @@
         <v>4</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>67</v>
+        <v>25</v>
       </c>
       <c r="E15" s="1">
         <v>1</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="G15" s="1">
         <v>0</v>
       </c>
       <c r="H15" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>46</v>
+        <v>65</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
-        <v>5</v>
+        <v>36</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>48</v>
+        <v>4</v>
       </c>
       <c r="C16" s="1">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>28</v>
+        <v>58</v>
       </c>
       <c r="E16" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="G16" s="1">
         <v>0</v>
       </c>
       <c r="H16" s="1">
-        <v>1</v>
-      </c>
-      <c r="I16" s="2"/>
+        <v>0</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
-        <v>40</v>
+        <v>5</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>6</v>
+        <v>41</v>
       </c>
       <c r="C17" s="1">
-        <v>4.5</v>
+        <v>12</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>67</v>
+        <v>25</v>
       </c>
       <c r="E17" s="1">
         <v>2</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="G17" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H17" s="1">
         <v>1</v>
       </c>
-      <c r="I17" s="2" t="s">
-        <v>46</v>
-      </c>
+      <c r="I17" s="2"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>6</v>
@@ -2119,10 +2178,10 @@
         <v>4.5</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="E18" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>56</v>
@@ -2134,27 +2193,27 @@
         <v>1</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>46</v>
+        <v>65</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C19" s="1">
-        <v>5</v>
+        <v>4.5</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>28</v>
+        <v>58</v>
       </c>
       <c r="E19" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>66</v>
+        <v>49</v>
       </c>
       <c r="G19" s="1">
         <v>1</v>
@@ -2162,29 +2221,31 @@
       <c r="H19" s="1">
         <v>1</v>
       </c>
-      <c r="I19" s="2"/>
+      <c r="I19" s="2" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>49</v>
+        <v>7</v>
       </c>
       <c r="C20" s="1">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E20" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="G20" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H20" s="1">
         <v>1</v>
@@ -2193,22 +2254,22 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
-        <v>44</v>
+        <v>8</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>7</v>
+        <v>42</v>
       </c>
       <c r="C21" s="1">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E21" s="1">
         <v>2</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="G21" s="1">
         <v>1</v>
@@ -2216,9 +2277,18 @@
       <c r="H21" s="1">
         <v>1</v>
       </c>
-      <c r="I21" s="2" t="s">
-        <v>45</v>
-      </c>
+      <c r="I21" s="2"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A22" s="1"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
+      <c r="I22" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2239,7 +2309,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -2262,15 +2332,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="B1" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B2">
         <v>8</v>

</xml_diff>